<commit_message>
updated test case id in reports, gitignored traces folder
</commit_message>
<xml_diff>
--- a/reports/sample_cases_report.xlsx
+++ b/reports/sample_cases_report.xlsx
@@ -530,7 +530,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_001</t>
+          <t>TC_001</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -579,7 +579,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_002</t>
+          <t>TC_002</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_003</t>
+          <t>TC_003</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_004</t>
+          <t>TC_004</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -728,7 +728,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_005</t>
+          <t>TC_005</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -777,7 +777,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_006</t>
+          <t>TC_006</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_007</t>
+          <t>TC_007</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_008</t>
+          <t>TC_008</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_009</t>
+          <t>TC_009</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -974,7 +974,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_010</t>
+          <t>TC_010</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_011</t>
+          <t>TC_011</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_012</t>
+          <t>TC_012</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_013</t>
+          <t>TC_013</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_014</t>
+          <t>TC_014</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_015</t>
+          <t>TC_015</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_016</t>
+          <t>TC_016</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_017</t>
+          <t>TC_017</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_018</t>
+          <t>TC_018</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_019</t>
+          <t>TC_019</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>TC_SAMPLE_CASES_020</t>
+          <t>TC_020</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">

</xml_diff>